<commit_message>
reglamento clase 2 carshow
</commit_message>
<xml_diff>
--- a/pista/TZ/kilos para el campeonato 2021.xlsx
+++ b/pista/TZ/kilos para el campeonato 2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lisandro\Desktop\FAPCDMS\Reglamentos\git\pista\TZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947D5A9A-5F21-4F52-B3C2-8EB13604E36B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B9D43B5-3C64-4183-8AEB-08793AF8FE5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{E2BB2F36-0BD4-400D-B47E-556235095EB9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E2BB2F36-0BD4-400D-B47E-556235095EB9}"/>
   </bookViews>
   <sheets>
     <sheet name="TZ 1600" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
   <si>
     <t>kilos para el campeonato 2021</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>OLIVERA, Gustavo</t>
+  </si>
+  <si>
+    <t>GIORGIS, Lucas</t>
   </si>
 </sst>
 </file>
@@ -319,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -340,6 +343,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -654,10 +658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7B3844A-ACA0-4468-AE6C-CF94B793A95E}">
-  <dimension ref="B3:I15"/>
+  <dimension ref="B3:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,7 +737,7 @@
       <c r="G6" s="7"/>
       <c r="H6" s="8"/>
       <c r="I6" s="7">
-        <f t="shared" ref="I6:I15" si="0">SUM(D6:H6)</f>
+        <f>SUM(D6:H6)</f>
         <v>45</v>
       </c>
     </row>
@@ -750,165 +754,204 @@
       <c r="E7" s="7">
         <v>15</v>
       </c>
-      <c r="F7" s="7"/>
+      <c r="F7" s="7">
+        <v>5</v>
+      </c>
       <c r="G7" s="7"/>
       <c r="H7" s="8"/>
       <c r="I7" s="7">
-        <f t="shared" si="0"/>
-        <v>40</v>
+        <f>SUM(D7:H7)</f>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="7"/>
+        <v>15</v>
+      </c>
+      <c r="D8" s="7">
+        <v>10</v>
+      </c>
       <c r="E8" s="7">
-        <v>20</v>
-      </c>
-      <c r="F8" s="7"/>
+        <v>5</v>
+      </c>
+      <c r="F8" s="7">
+        <v>25</v>
+      </c>
       <c r="G8" s="7"/>
       <c r="H8" s="8"/>
       <c r="I8" s="7">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <f>SUM(D8:H8)</f>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="7">
-        <v>15</v>
-      </c>
-      <c r="E9" s="7"/>
+        <v>18</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7">
+        <v>20</v>
+      </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="8"/>
       <c r="I9" s="7">
-        <f t="shared" si="0"/>
-        <v>15</v>
+        <f>SUM(D9:H9)</f>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="7">
-        <v>10</v>
-      </c>
-      <c r="E10" s="7">
-        <v>5</v>
-      </c>
-      <c r="F10" s="7"/>
+        <v>17</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7">
+        <v>20</v>
+      </c>
       <c r="G10" s="7"/>
       <c r="H10" s="8"/>
       <c r="I10" s="7">
-        <f t="shared" si="0"/>
-        <v>15</v>
+        <f>SUM(D10:H10)</f>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7">
-        <v>10</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D11" s="7">
+        <v>15</v>
+      </c>
+      <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="8"/>
       <c r="I11" s="7">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <f>SUM(D11:H11)</f>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="7">
-        <v>10</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="7">
-        <v>5</v>
-      </c>
+      <c r="B12" s="16">
+        <v>24</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="7"/>
       <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+      <c r="F12" s="7">
+        <v>15</v>
+      </c>
       <c r="G12" s="7"/>
       <c r="H12" s="8"/>
       <c r="I12" s="7">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>SUM(D12:H12)</f>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="7">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
+      <c r="F13" s="7">
+        <v>10</v>
+      </c>
       <c r="G13" s="7"/>
       <c r="H13" s="8"/>
       <c r="I13" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>SUM(D13:H13)</f>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="7">
-        <v>117</v>
+        <v>10</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="7"/>
+        <v>16</v>
+      </c>
+      <c r="D14" s="7">
+        <v>5</v>
+      </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="8"/>
       <c r="I14" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>SUM(D14:H14)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="7">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
+      <c r="E15" s="7">
+        <v>10</v>
+      </c>
+      <c r="F15" s="7">
+        <v>-10</v>
+      </c>
       <c r="G15" s="7"/>
       <c r="H15" s="8"/>
       <c r="I15" s="7">
-        <f t="shared" si="0"/>
+        <f>SUM(D15:H15)</f>
         <v>0</v>
       </c>
     </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="7">
+        <v>117</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7">
+        <f>SUM(D16:H16)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B6:I15">
-    <sortCondition descending="1" ref="I6:I15"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B6:I17">
+    <sortCondition descending="1" ref="I6:I17"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -919,8 +962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E8A25B-0A4D-45A3-9827-271453EC9EE3}">
   <dimension ref="B3:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -981,23 +1024,25 @@
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="7">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" s="7">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E6" s="7">
-        <v>20</v>
-      </c>
-      <c r="F6" s="7"/>
+        <v>10</v>
+      </c>
+      <c r="F6" s="7">
+        <v>25</v>
+      </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7">
-        <f>SUM(D6:E6)</f>
-        <v>35</v>
+        <f>SUM(D6:H6)-5</f>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
@@ -1013,33 +1058,35 @@
       <c r="E7" s="7">
         <v>25</v>
       </c>
-      <c r="F7" s="7"/>
+      <c r="F7" s="7">
+        <v>-5</v>
+      </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7">
         <f>SUM(D7:H7)</f>
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
-        <v>69</v>
+        <v>12</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D8" s="7">
+        <v>5</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7">
         <v>20</v>
       </c>
-      <c r="E8" s="7">
-        <v>10</v>
-      </c>
-      <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7">
-        <f>SUM(D8,E8)</f>
-        <v>30</v>
+        <f>SUM(D8:H8)</f>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
@@ -1059,7 +1106,7 @@
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7">
-        <f>SUM(D9,E9)</f>
+        <f>SUM(D9:H9)</f>
         <v>20</v>
       </c>
     </row>
@@ -1084,40 +1131,44 @@
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="7">
-        <v>5</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="D11" s="7"/>
       <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
+      <c r="F11" s="7">
+        <v>15</v>
+      </c>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7">
         <f>SUM(D11:H11)</f>
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="7"/>
+        <v>24</v>
+      </c>
+      <c r="D12" s="7">
+        <v>15</v>
+      </c>
       <c r="E12" s="7">
-        <v>5</v>
-      </c>
-      <c r="F12" s="7"/>
+        <v>20</v>
+      </c>
+      <c r="F12" s="7">
+        <v>-25</v>
+      </c>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7">
         <f>SUM(D12:H12)</f>
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
@@ -1129,45 +1180,60 @@
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
+      <c r="F13" s="7">
+        <v>10</v>
+      </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
+      <c r="I13" s="7">
+        <f>SUM(D13:H13)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="7">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
+      <c r="E14" s="7">
+        <v>5</v>
+      </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
+      <c r="I14" s="7">
+        <f>SUM(D14:H14)</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="7">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
+      <c r="F15" s="7">
+        <v>5</v>
+      </c>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
+      <c r="I15" s="7">
+        <f>SUM(D15:H15)</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="7">
-        <v>222</v>
+        <v>3</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
@@ -1178,10 +1244,10 @@
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="7">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
@@ -1192,10 +1258,10 @@
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="7">
-        <v>29</v>
+        <v>222</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
@@ -1206,10 +1272,10 @@
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="7">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
@@ -1220,10 +1286,10 @@
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="7">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
@@ -1234,10 +1300,10 @@
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="7">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>

</xml_diff>